<commit_message>
First prep room order
Created
- order tracking spreadsheet
- prep room order template
- prep room order 1
</commit_message>
<xml_diff>
--- a/orders/prep-room/ProjectSuppliesRequestForm_FLoRaCommunications_Order1.xlsx
+++ b/orders/prep-room/ProjectSuppliesRequestForm_FLoRaCommunications_Order1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a8a7dff0b441a3a2/Documents/GitHub/flora-hardware/orders/prep-room/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4629AEBE-49BD-4929-B70D-2AADF6D99FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99B027F6-530C-4E10-B308-4307FE1B26FB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4629AEBE-49BD-4929-B70D-2AADF6D99FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{872632FD-1AB2-4DFA-B0A2-DD77F216447E}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,6 +746,15 @@
     <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="3" fillId="4" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -764,6 +773,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -778,18 +790,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1109,8 +1109,8 @@
   </sheetPr>
   <dimension ref="A2:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1128,31 +1128,31 @@
   <sheetData>
     <row r="2" spans="1:13" ht="24" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A2" s="1"/>
-      <c r="B2" s="73" t="s">
+      <c r="B2" s="77" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="73"/>
-      <c r="D2" s="73"/>
-      <c r="E2" s="73"/>
-      <c r="F2" s="73"/>
-      <c r="G2" s="73"/>
-      <c r="H2" s="73"/>
-      <c r="I2" s="73"/>
-      <c r="J2" s="73"/>
-      <c r="K2" s="73"/>
-      <c r="L2" s="73"/>
-      <c r="M2" s="73"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
+      <c r="H2" s="77"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="77"/>
+      <c r="K2" s="77"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="77"/>
     </row>
     <row r="3" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A3" s="1"/>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="76" t="s">
+      <c r="C3" s="78"/>
+      <c r="D3" s="80" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="77"/>
+      <c r="E3" s="81"/>
       <c r="F3" s="56" t="s">
         <v>16</v>
       </c>
@@ -1162,20 +1162,20 @@
       <c r="H3" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="70" t="s">
+      <c r="I3" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-      <c r="L3" s="71"/>
-      <c r="M3" s="72"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="75"/>
     </row>
     <row r="4" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A4" s="1"/>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="75"/>
+      <c r="C4" s="79"/>
       <c r="D4" s="41">
         <f ca="1">TODAY()</f>
         <v>45551</v>
@@ -1186,13 +1186,13 @@
       <c r="H4" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="I4" s="80" t="s">
+      <c r="I4" s="76" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
-      <c r="M4" s="72"/>
+      <c r="J4" s="74"/>
+      <c r="K4" s="74"/>
+      <c r="L4" s="74"/>
+      <c r="M4" s="75"/>
     </row>
     <row r="5" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="A5" s="1"/>
@@ -1222,11 +1222,11 @@
       <c r="H6" s="9"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
-      <c r="K6" s="67" t="s">
+      <c r="K6" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="L6" s="68"/>
-      <c r="M6" s="69"/>
+      <c r="L6" s="71"/>
+      <c r="M6" s="72"/>
     </row>
     <row r="7" spans="1:13" ht="66.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="20" t="s">
@@ -1276,10 +1276,10 @@
       <c r="B8" s="42">
         <v>4</v>
       </c>
-      <c r="C8" s="79" t="s">
+      <c r="C8" s="68" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="78">
+      <c r="D8" s="67">
         <v>20855</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1288,7 +1288,7 @@
       <c r="F8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="81" t="s">
+      <c r="G8" s="69" t="s">
         <v>30</v>
       </c>
       <c r="H8" s="10" t="s">
@@ -1297,7 +1297,10 @@
       <c r="I8" s="32">
         <v>10.39</v>
       </c>
-      <c r="J8" s="64"/>
+      <c r="J8" s="64">
+        <f>I8*B8</f>
+        <v>41.56</v>
+      </c>
       <c r="K8" s="59"/>
       <c r="L8" s="34"/>
       <c r="M8" s="35"/>
@@ -2149,7 +2152,7 @@
       <c r="I58" s="54"/>
       <c r="J58" s="54">
         <f>SUM(J8:J57)</f>
-        <v>0</v>
+        <v>41.56</v>
       </c>
       <c r="K58" s="53"/>
       <c r="L58" s="27"/>

</xml_diff>